<commit_message>
spreadsheets: Fixed bug in organisation spreadsheet
Contents from one column were not being picked up due to incorrect field name
</commit_message>
<xml_diff>
--- a/indigo/spreadsheetform_guides/organisation_v005.xlsx
+++ b/indigo/spreadsheetform_guides/organisation_v005.xlsx
@@ -197,7 +197,7 @@
     <t xml:space="preserve">Notes</t>
   </si>
   <si>
-    <t xml:space="preserve">SPREADSHEETFORM:DOWN:org-ids/secondary:org-id/value</t>
+    <t xml:space="preserve">SPREADSHEETFORM:DOWN:org-ids/secondary:organisation_id/value</t>
   </si>
   <si>
     <t xml:space="preserve">SPREADSHEETFORM:DOWN:org-ids/secondary:source_ids</t>
@@ -1465,12 +1465,12 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -1536,7 +1536,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -1546,12 +1546,11 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="34.35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="34.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="18.47"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="11.54"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1592,7 +1591,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -1602,13 +1601,12 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="42.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="67.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="49.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="22.62"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="11.54"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1840,7 +1838,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -1850,12 +1848,11 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="37.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="49.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="27.23"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="11.54"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2050,7 +2047,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -2060,12 +2057,11 @@
       <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.86"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="11.54"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2252,7 +2248,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -2262,16 +2258,13 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="1" style="0" width="11.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="30.02"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="11.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="17.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="17.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="19.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="19.31"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="10" style="0" width="11.54"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2671,7 +2664,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -2681,10 +2674,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.54"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -3618,7 +3608,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -3628,10 +3618,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.54"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -4890,7 +4877,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -4900,10 +4887,9 @@
       <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.23"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="11.54"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>